<commit_message>
update 3502 and 3506 IO
</commit_message>
<xml_diff>
--- a/MIR3502/MIR3502-3506端口对比表.xlsx
+++ b/MIR3502/MIR3502-3506端口对比表.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="管脚对比" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterate="1" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="139">
   <si>
     <t>IMR3502 插座C</t>
   </si>
@@ -161,9 +161,6 @@
     </r>
   </si>
   <si>
-    <t>AI-06</t>
-  </si>
-  <si>
     <t>DI_06</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     </r>
   </si>
   <si>
-    <t>AI-07</t>
-  </si>
-  <si>
     <t>DI_07</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
     </r>
   </si>
   <si>
-    <t>AI-08</t>
-  </si>
-  <si>
     <t>DI_08</t>
   </si>
   <si>
@@ -272,9 +263,6 @@
     <t>4:</t>
   </si>
   <si>
-    <t>AI-09</t>
-  </si>
-  <si>
     <t>DI_09</t>
   </si>
   <si>
@@ -287,9 +275,6 @@
     <t>5:</t>
   </si>
   <si>
-    <t>AI-10</t>
-  </si>
-  <si>
     <t>DI_10</t>
   </si>
   <si>
@@ -302,9 +287,6 @@
     <t>6:</t>
   </si>
   <si>
-    <t>AI-11</t>
-  </si>
-  <si>
     <t>DI_11</t>
   </si>
   <si>
@@ -317,9 +299,6 @@
     <t>7:</t>
   </si>
   <si>
-    <t>AI-12</t>
-  </si>
-  <si>
     <t>DI_12</t>
   </si>
   <si>
@@ -332,9 +311,6 @@
     <t>8:</t>
   </si>
   <si>
-    <t>AI-13</t>
-  </si>
-  <si>
     <t>DI_13</t>
   </si>
   <si>
@@ -347,9 +323,6 @@
     <t>9:</t>
   </si>
   <si>
-    <t>AI-14</t>
-  </si>
-  <si>
     <t>DI_14</t>
   </si>
   <si>
@@ -362,9 +335,6 @@
     <t>10:</t>
   </si>
   <si>
-    <t>AI-15</t>
-  </si>
-  <si>
     <t>DI_15</t>
   </si>
   <si>
@@ -377,9 +347,6 @@
     <t>11:</t>
   </si>
   <si>
-    <t>AI-16</t>
-  </si>
-  <si>
     <t>DI_16</t>
   </si>
   <si>
@@ -392,9 +359,6 @@
     <t>12:</t>
   </si>
   <si>
-    <t>AI-17</t>
-  </si>
-  <si>
     <t>DI_17</t>
   </si>
   <si>
@@ -494,9 +458,6 @@
     <t>24:</t>
   </si>
   <si>
-    <t>AI-29</t>
-  </si>
-  <si>
     <t>DI_29</t>
   </si>
   <si>
@@ -512,9 +473,6 @@
     <t>25:</t>
   </si>
   <si>
-    <t>AI-28</t>
-  </si>
-  <si>
     <t>DI_28</t>
   </si>
   <si>
@@ -527,9 +485,6 @@
     <t>26:</t>
   </si>
   <si>
-    <t>AI-27</t>
-  </si>
-  <si>
     <t>DI_27</t>
   </si>
   <si>
@@ -542,9 +497,6 @@
     <t>27:</t>
   </si>
   <si>
-    <t>AI-26</t>
-  </si>
-  <si>
     <t>DI_26</t>
   </si>
   <si>
@@ -557,9 +509,6 @@
     <t>28:</t>
   </si>
   <si>
-    <t>AI-25</t>
-  </si>
-  <si>
     <t>DI_25</t>
   </si>
   <si>
@@ -572,9 +521,6 @@
     <t>29:</t>
   </si>
   <si>
-    <t>AI-24</t>
-  </si>
-  <si>
     <t>DI_24</t>
   </si>
   <si>
@@ -587,9 +533,6 @@
     <t>30:</t>
   </si>
   <si>
-    <t>AI-23</t>
-  </si>
-  <si>
     <t>DI_23</t>
   </si>
   <si>
@@ -602,9 +545,6 @@
     <t>31:</t>
   </si>
   <si>
-    <t>AI-22</t>
-  </si>
-  <si>
     <t>DI_22</t>
   </si>
   <si>
@@ -617,9 +557,6 @@
     <t>32:</t>
   </si>
   <si>
-    <t>AI-21</t>
-  </si>
-  <si>
     <t>DI_21</t>
   </si>
   <si>
@@ -632,9 +569,6 @@
     <t>33:</t>
   </si>
   <si>
-    <t>AI-20</t>
-  </si>
-  <si>
     <t>DI_20</t>
   </si>
   <si>
@@ -647,9 +581,6 @@
     <t>34:</t>
   </si>
   <si>
-    <t>AI-19</t>
-  </si>
-  <si>
     <t>DI_19</t>
   </si>
   <si>
@@ -660,9 +591,6 @@
   </si>
   <si>
     <t>35:</t>
-  </si>
-  <si>
-    <t>AI-18</t>
   </si>
   <si>
     <t>DI_18</t>
@@ -682,9 +610,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -734,7 +662,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -742,6 +670,44 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -765,54 +731,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -826,8 +753,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -840,16 +775,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -857,13 +785,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,49 +800,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -926,133 +974,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1131,15 +1065,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1151,6 +1076,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1183,152 +1117,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1340,7 +1274,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1675,7 +1610,7 @@
   <dimension ref="D1:R65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1742,1189 +1677,1141 @@
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="4" t="s">
-        <v>16</v>
+      <c r="R3" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="4:18">
       <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="4" t="s">
-        <v>16</v>
+      <c r="R4" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="4:18">
       <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="4" t="s">
-        <v>16</v>
+      <c r="R5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="4:18">
       <c r="D6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4" t="s">
-        <v>16</v>
+      <c r="R6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="4:18">
       <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="s">
-        <v>16</v>
+      <c r="R7" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="4:18">
       <c r="D8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="4" t="s">
-        <v>16</v>
+      <c r="R8" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="4:18">
       <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4" t="s">
-        <v>16</v>
+      <c r="R9" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="4:18">
       <c r="D10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
-        <v>16</v>
+      <c r="R10" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="4:18">
       <c r="D11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4" t="s">
-        <v>16</v>
+      <c r="R11" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="4:18">
       <c r="D12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="s">
-        <v>16</v>
+      <c r="R12" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="4:18">
       <c r="D13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4" t="s">
-        <v>16</v>
+      <c r="R13" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="4:18">
       <c r="D14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4" t="s">
-        <v>16</v>
+      <c r="R14" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="4:18">
       <c r="D15" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="J15" s="4"/>
       <c r="L15" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="4:18">
       <c r="D16" s="4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="J16" s="4"/>
       <c r="L16" s="4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="4:18">
       <c r="D17" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="4:18">
       <c r="D18" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="4:18">
       <c r="D19" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="4:18">
       <c r="D20" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="4:18">
       <c r="D21" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N21" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="4:18">
       <c r="D22" s="4" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="4:18">
       <c r="D23" s="4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="J23" s="4"/>
       <c r="L23" s="4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="R23" s="4"/>
     </row>
     <row r="24" spans="4:18">
       <c r="D24" s="4" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J24" s="4"/>
       <c r="L24" s="4" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="R24" s="4"/>
     </row>
     <row r="25" spans="4:18">
       <c r="D25" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J25" s="4"/>
       <c r="L25" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="R25" s="4"/>
     </row>
     <row r="26" ht="15" customHeight="1" spans="4:18">
       <c r="D26" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>102</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
       <c r="Q26" s="4"/>
-      <c r="R26" s="4" t="s">
-        <v>16</v>
+      <c r="R26" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="4:18">
       <c r="D27" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>108</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H27" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="O27" s="9"/>
-      <c r="P27" s="10"/>
+        <v>97</v>
+      </c>
+      <c r="O27" s="10"/>
+      <c r="P27" s="11"/>
       <c r="Q27" s="4"/>
-      <c r="R27" s="4" t="s">
-        <v>16</v>
+      <c r="R27" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="4:18">
       <c r="D28" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>113</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" s="4"/>
+        <v>99</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="5"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="O28" s="9"/>
-      <c r="P28" s="10"/>
+        <v>101</v>
+      </c>
+      <c r="O28" s="10"/>
+      <c r="P28" s="11"/>
       <c r="Q28" s="4"/>
-      <c r="R28" s="4" t="s">
-        <v>16</v>
+      <c r="R28" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="4:18">
       <c r="D29" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>118</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H29" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H29" s="5"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
       <c r="Q29" s="4"/>
-      <c r="R29" s="4" t="s">
-        <v>16</v>
+      <c r="R29" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="4:18">
       <c r="D30" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H30" s="4"/>
+        <v>107</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="5"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
+        <v>109</v>
+      </c>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
       <c r="Q30" s="4"/>
-      <c r="R30" s="4" t="s">
-        <v>16</v>
+      <c r="R30" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="4:18">
       <c r="D31" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>128</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H31" s="4"/>
+        <v>111</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" s="5"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
+        <v>113</v>
+      </c>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="4" t="s">
-        <v>16</v>
+      <c r="R31" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="4:18">
       <c r="D32" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>133</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="H32" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" s="5"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
+        <v>117</v>
+      </c>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="4" t="s">
-        <v>16</v>
+      <c r="R32" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="4:18">
       <c r="D33" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>138</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="H33" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H33" s="5"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
+        <v>121</v>
+      </c>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
       <c r="Q33" s="4"/>
-      <c r="R33" s="4" t="s">
-        <v>16</v>
+      <c r="R33" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="4:18">
       <c r="D34" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>143</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="H34" s="4"/>
+        <v>123</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="5"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="4" t="s">
-        <v>16</v>
+        <v>125</v>
+      </c>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="4:18">
       <c r="D35" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>148</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H35" s="4"/>
+        <v>127</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" s="5"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="K35" s="8"/>
       <c r="L35" s="4" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
+        <v>129</v>
+      </c>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
       <c r="Q35" s="4"/>
-      <c r="R35" s="4" t="s">
-        <v>16</v>
+      <c r="R35" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="4:18">
       <c r="D36" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>153</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H36" s="4"/>
+        <v>131</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" s="5"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K36" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="K36" s="8"/>
       <c r="L36" s="4" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
+        <v>133</v>
+      </c>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
       <c r="Q36" s="4"/>
-      <c r="R36" s="4" t="s">
-        <v>16</v>
+      <c r="R36" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="4:18">
       <c r="D37" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>158</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>161</v>
+        <v>135</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K37" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="K37" s="8"/>
       <c r="L37" s="4" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
+        <v>138</v>
+      </c>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="4" t="s">
-        <v>16</v>
+      <c r="R37" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="11:11">
-      <c r="K38" s="7"/>
+      <c r="K38" s="8"/>
     </row>
     <row r="56" spans="6:10">
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
     </row>
     <row r="57" spans="6:10">
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="6"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="7"/>
     </row>
     <row r="58" spans="6:10">
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
     </row>
     <row r="59" spans="6:10">
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
     </row>
     <row r="60" spans="6:10">
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
     </row>
     <row r="61" spans="6:10">
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
     </row>
     <row r="62" spans="6:10">
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
     </row>
     <row r="63" spans="6:10">
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
     </row>
     <row r="64" spans="6:10">
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
-      <c r="I64" s="7"/>
-      <c r="J64" s="7"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
     </row>
     <row r="65" spans="6:10">
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>